<commit_message>
Major refactoring n1: merged planet object and space object classes. Added some english texts
</commit_message>
<xml_diff>
--- a/doc/������ �����������.xlsx
+++ b/doc/������ �����������.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
@@ -11,12 +11,12 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Объем текста в КБ</t>
   </si>
@@ -32,12 +32,21 @@
   <si>
     <t>Файлы</t>
   </si>
+  <si>
+    <t>21.25</t>
+  </si>
+  <si>
+    <t>42.5</t>
+  </si>
+  <si>
+    <t>Диалоги martan1, first_press_conference, первый диалог с Садовником и диалог с Гордоном перед ним</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,7 +168,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -194,7 +202,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -370,14 +377,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" style="1" customWidth="1"/>
@@ -385,7 +392,7 @@
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -399,7 +406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -411,6 +418,20 @@
       </c>
       <c r="D2" s="2">
         <v>41843</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2">
+        <v>41850</v>
       </c>
     </row>
   </sheetData>
@@ -420,24 +441,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added descriptions for homeworlds
</commit_message>
<xml_diff>
--- a/doc/������ �����������.xlsx
+++ b/doc/������ �����������.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Объем текста в КБ</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Диалоги martan1, first_press_conference, первый диалог с Садовником и диалог с Гордоном перед ним</t>
+  </si>
+  <si>
+    <t>Страница about блога, клиск_торговля</t>
   </si>
 </sst>
 </file>
@@ -378,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -434,6 +437,20 @@
         <v>41850</v>
       </c>
     </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="C4">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="D4" s="2">
+        <v>41863</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Removed some old dialogs. Added 2 new pictures
</commit_message>
<xml_diff>
--- a/doc/������ �����������.xlsx
+++ b/doc/������ �����������.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Объем текста в КБ</t>
   </si>
@@ -49,6 +49,15 @@
 Второй диалог Мартан ПОСЛЕ ОБСУЖДЕНИЯ ЭКАУНТЕРОВ
 martan_default
 </t>
+  </si>
+  <si>
+    <t>Борки посольство испытание</t>
+  </si>
+  <si>
+    <t>Оплачено, руб</t>
+  </si>
+  <si>
+    <t>Три поста в блоге (хелловорлд, о сюжете, о геймплее)</t>
   </si>
 </sst>
 </file>
@@ -390,21 +399,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="3" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -415,10 +424,13 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -428,11 +440,11 @@
       <c r="C2">
         <v>7</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>41843</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -442,11 +454,11 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>41850</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -456,11 +468,11 @@
       <c r="C4">
         <v>34.200000000000003</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>41863</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="75">
+    <row r="5" spans="1:5" ht="75">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -470,8 +482,24 @@
       <c r="C5">
         <v>194.8</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>41943</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1">
+        <v>8.6999999999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to latest Frankenstein library version
</commit_message>
<xml_diff>
--- a/doc/������ �����������.xlsx
+++ b/doc/������ �����������.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Объем текста в КБ</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Пост про алиенов</t>
+  </si>
+  <si>
+    <t>3 диалога tutorials + research и некоторые иные properties</t>
   </si>
 </sst>
 </file>
@@ -402,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -525,6 +528,20 @@
         <v>41987</v>
       </c>
     </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1">
+        <v>23.4</v>
+      </c>
+      <c r="D11">
+        <v>1638</v>
+      </c>
+      <c r="E11" s="2">
+        <v>41990</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Trade screen looking good
</commit_message>
<xml_diff>
--- a/doc/������ �����������.xlsx
+++ b/doc/������ �����������.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Объем текста в КБ</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>3 диалога tutorials + research и некоторые иные properties</t>
+  </si>
+  <si>
+    <t>journal, help, gameover</t>
+  </si>
+  <si>
+    <t>private_messages</t>
   </si>
 </sst>
 </file>
@@ -405,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -540,6 +546,34 @@
       </c>
       <c r="E11" s="2">
         <v>41990</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1">
+        <v>49</v>
+      </c>
+      <c r="D12">
+        <v>3430</v>
+      </c>
+      <c r="E12" s="2">
+        <v>42002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1">
+        <v>18</v>
+      </c>
+      <c r="D13">
+        <v>1260</v>
+      </c>
+      <c r="E13" s="2">
+        <v>42002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a record in zorsan rebels quest that notifies that there is no continuation. Fixed bug with incorrect lost crew score.
</commit_message>
<xml_diff>
--- a/doc/������ �����������.xlsx
+++ b/doc/������ �����������.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Переводы" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Объем текста в КБ</t>
   </si>
@@ -73,6 +73,36 @@
   </si>
   <si>
     <t>Пост в блоге о greenlight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дата </t>
+  </si>
+  <si>
+    <t>Сумма</t>
+  </si>
+  <si>
+    <t>Номер перевода</t>
+  </si>
+  <si>
+    <t>Платежная система</t>
+  </si>
+  <si>
+    <t>Сбербанк</t>
+  </si>
+  <si>
+    <t>Колибри</t>
+  </si>
+  <si>
+    <t>Контакт</t>
+  </si>
+  <si>
+    <t>"за книги"</t>
+  </si>
+  <si>
+    <t>Юнистрим</t>
+  </si>
+  <si>
+    <t>Итог:</t>
   </si>
 </sst>
 </file>
@@ -416,7 +446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -595,12 +625,147 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="33.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2">
+        <v>41983</v>
+      </c>
+      <c r="B2">
+        <v>5200</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2">
+        <v>41990</v>
+      </c>
+      <c r="B3">
+        <v>1638</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2">
+        <v>42002</v>
+      </c>
+      <c r="B4">
+        <v>3430</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2">
+        <v>42041</v>
+      </c>
+      <c r="B5">
+        <v>13000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5">
+        <v>134135705</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2">
+        <v>42064</v>
+      </c>
+      <c r="B6">
+        <v>6000</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>894220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2">
+        <v>42138</v>
+      </c>
+      <c r="B7">
+        <v>1300</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2">
+        <v>42265</v>
+      </c>
+      <c r="B8">
+        <v>8500</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8">
+        <v>9632894888</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2">
+        <v>42448</v>
+      </c>
+      <c r="B9">
+        <v>3700</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9">
+        <v>279029900289</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <f>SUM(B2:B16)</f>
+        <v>42768</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>